<commit_message>
Atualizando as sprints e adicionando o diagrama de caso de uso de relatorio
</commit_message>
<xml_diff>
--- a/SCRUM/Planilha de Sprints.xlsx
+++ b/SCRUM/Planilha de Sprints.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACE2CD3-7D71-4382-B5E3-CF19E68207B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CFBC1A-E870-44BD-BD76-5ABB0F0495DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="61">
   <si>
     <t>Tarefa</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Planilha de testes</t>
-  </si>
-  <si>
-    <t>Criar relatórios para gestão</t>
   </si>
   <si>
     <t>Separar os requisitos (Backlog)</t>
@@ -186,9 +183,6 @@
     <t>Desenvolver os Diagramas de Classes</t>
   </si>
   <si>
-    <t>Desenvolver telas restantes do protótipo</t>
-  </si>
-  <si>
     <t>Desenvolver interação das telas do protótipo</t>
   </si>
   <si>
@@ -198,16 +192,31 @@
     <t>Diagrama de caso de uso - Produtos</t>
   </si>
   <si>
-    <t>Em desenvolvimento</t>
-  </si>
-  <si>
-    <t>Desenvolver o Modelo de Entidade Relacionamento</t>
-  </si>
-  <si>
     <t>Desenvolver a tela de protótipo do Cliente</t>
   </si>
   <si>
     <t>Vitor</t>
+  </si>
+  <si>
+    <t>Desenvolver o Diagrama de Entidade Relacionamento</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Desenvolver tela de Produto</t>
+  </si>
+  <si>
+    <t>Desenvolver tela de configuração</t>
+  </si>
+  <si>
+    <t>Finalização da tela do PoC (CRUD)</t>
+  </si>
+  <si>
+    <t>Criar o código de criação da Database</t>
+  </si>
+  <si>
+    <t>Diagrama de caso de uso - Geral</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1196,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1352,6 +1361,9 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="40" borderId="15" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1361,8 +1373,32 @@
     <xf numFmtId="0" fontId="38" fillId="40" borderId="17" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="28" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="28" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="42" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -3272,6 +3308,108 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>678542</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>222249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>695008</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>262130</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 1" descr="Weekly Chore Schedule" title="Title 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{509B528E-FE47-4591-A328-7553C49047E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2043792" y="11556999"/>
+          <a:ext cx="30988591" cy="579631"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Corbel" panose="020B0503020204020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Bahnschrift" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>SPRINT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Bahnschrift" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> 7 (12/05 a 18/05)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2400">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Bahnschrift" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3300,7 +3438,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela3" displayName="Tabela3" ref="D44:D45" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10" dataCellStyle="Hiperlink">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela3" displayName="Tabela3" ref="D51:D52" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10" dataCellStyle="Hiperlink">
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="GitHub" dataDxfId="9" dataCellStyle="Hiperlink"/>
   </tableColumns>
@@ -3309,7 +3447,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabela9" displayName="Tabela9" ref="D48:G54" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabela9" displayName="Tabela9" ref="D55:G61" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4" headerRowCellStyle="Normal 2">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Nome" dataDxfId="3" dataCellStyle="Normal 2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Turma" dataDxfId="2" dataCellStyle="Normal 2"/>
@@ -3526,10 +3664,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="D1:T54"/>
+  <dimension ref="D1:T61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" customHeight="1"/>
@@ -3632,7 +3770,7 @@
     </row>
     <row r="5" spans="4:20" ht="21" customHeight="1">
       <c r="D5" s="50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>5</v>
@@ -3657,7 +3795,7 @@
     </row>
     <row r="6" spans="4:20" ht="21" customHeight="1">
       <c r="D6" s="50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>11</v>
@@ -3733,7 +3871,7 @@
     </row>
     <row r="11" spans="4:20" ht="21" customHeight="1">
       <c r="D11" s="50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>10</v>
@@ -3868,7 +4006,7 @@
     </row>
     <row r="18" spans="4:18" ht="21" customHeight="1">
       <c r="D18" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="28" t="s">
         <v>5</v>
@@ -3882,10 +4020,10 @@
     </row>
     <row r="19" spans="4:18" ht="21" customHeight="1">
       <c r="D19" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>2</v>
@@ -3896,10 +4034,10 @@
     </row>
     <row r="20" spans="4:18" ht="21" customHeight="1">
       <c r="D20" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>2</v>
@@ -3910,7 +4048,7 @@
     </row>
     <row r="21" spans="4:18" ht="21" customHeight="1">
       <c r="D21" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" s="22" t="s">
         <v>8</v>
@@ -3924,7 +4062,7 @@
     </row>
     <row r="22" spans="4:18" ht="21" customHeight="1">
       <c r="D22" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>11</v>
@@ -3977,13 +4115,13 @@
     </row>
     <row r="27" spans="4:18" ht="21" customHeight="1">
       <c r="D27" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>14</v>
@@ -3991,13 +4129,13 @@
     </row>
     <row r="28" spans="4:18" ht="21" customHeight="1">
       <c r="D28" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="59" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+      <c r="E28" s="56" t="s">
+        <v>53</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>6</v>
@@ -4015,13 +4153,13 @@
     </row>
     <row r="29" spans="4:18" ht="21" customHeight="1">
       <c r="D29" s="27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>5</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G29" s="28" t="s">
         <v>6</v>
@@ -4071,7 +4209,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>14</v>
@@ -4079,13 +4217,13 @@
     </row>
     <row r="35" spans="4:18" ht="21" customHeight="1">
       <c r="D35" s="29" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E35" s="22" t="s">
         <v>5</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G35" s="22" t="s">
         <v>6</v>
@@ -4128,186 +4266,272 @@
       </c>
     </row>
     <row r="40" spans="4:18" ht="21" customHeight="1">
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" ht="21" customHeight="1">
+      <c r="D41" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18" ht="21" customHeight="1">
+      <c r="D42" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F42" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="4:18" ht="21" customHeight="1">
+      <c r="D43" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" s="63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="4:18" ht="21" customHeight="1">
+      <c r="D44" s="64"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="67"/>
+    </row>
+    <row r="45" spans="4:18" ht="21" customHeight="1">
+      <c r="D45" s="60"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="63"/>
+    </row>
+    <row r="46" spans="4:18" ht="21" customHeight="1">
+      <c r="D46" s="60"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="63"/>
+    </row>
+    <row r="47" spans="4:18" ht="21" customHeight="1">
+      <c r="D47" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="4:18" ht="21" customHeight="1">
+      <c r="D48" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="4:18" ht="21" customHeight="1">
-      <c r="D41" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="20" t="s">
+      <c r="G48" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="4:18" ht="21" customHeight="1">
+      <c r="D49" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="E49" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F49" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="4:18" ht="21" customHeight="1">
-      <c r="D42" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="22" t="s">
+      <c r="G49" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="4:18" ht="21" customHeight="1">
-      <c r="D44" s="48" t="s">
+    <row r="50" spans="4:18" s="16" customFormat="1" ht="21" customHeight="1">
+      <c r="D50" s="68"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="R50" s="15"/>
+    </row>
+    <row r="51" spans="4:18" ht="21" customHeight="1">
+      <c r="D51" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="4"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="4:18" ht="21" customHeight="1">
+      <c r="D52" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="4:18" ht="21" customHeight="1">
-      <c r="D45" s="49" t="s">
+      <c r="E52" s="4"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="4"/>
+    </row>
+    <row r="54" spans="4:18" ht="21" customHeight="1">
+      <c r="D54" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="59"/>
+    </row>
+    <row r="55" spans="4:18" ht="21" customHeight="1">
+      <c r="D55" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="4"/>
-    </row>
-    <row r="47" spans="4:18" ht="21" customHeight="1">
-      <c r="D47" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="58"/>
-    </row>
-    <row r="48" spans="4:18" ht="21" customHeight="1">
-      <c r="D48" s="24" t="s">
+      <c r="E55" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="F55" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="25" t="s">
+      <c r="G55" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="4:18" ht="21" customHeight="1">
+      <c r="D56" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="G48" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="4:7" ht="21" customHeight="1">
-      <c r="D49" s="38" t="s">
+      <c r="E56" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="39" t="s">
+      <c r="F56" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F49" s="39" t="s">
+      <c r="G56" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="G49" s="40" t="s">
+    </row>
+    <row r="57" spans="4:18" ht="21" customHeight="1">
+      <c r="D57" s="38" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="50" spans="4:7" ht="21" customHeight="1">
-      <c r="D50" s="38" t="s">
+      <c r="E57" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E50" s="39" t="s">
+      <c r="F57" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F50" s="39" t="s">
+      <c r="G57" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="G50" s="41" t="s">
+    </row>
+    <row r="58" spans="4:18" ht="21" customHeight="1">
+      <c r="D58" s="38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="51" spans="4:7" ht="21" customHeight="1">
-      <c r="D51" s="38" t="s">
+      <c r="E58" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="E51" s="39" t="s">
+      <c r="F58" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="39" t="s">
+      <c r="G58" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="G51" s="41" t="s">
+    </row>
+    <row r="59" spans="4:18" ht="21" customHeight="1">
+      <c r="D59" s="38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="52" spans="4:7" ht="21" customHeight="1">
-      <c r="D52" s="38" t="s">
+      <c r="E59" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G59" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="G52" s="41" t="s">
+    </row>
+    <row r="60" spans="4:18" ht="21" customHeight="1">
+      <c r="D60" s="38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="4:7" ht="21" customHeight="1">
-      <c r="D53" s="38" t="s">
+      <c r="E60" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G60" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="E53" s="39" t="s">
+    </row>
+    <row r="61" spans="4:18" ht="21" customHeight="1">
+      <c r="D61" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="G53" s="41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="4:7" ht="21" customHeight="1">
-      <c r="D54" s="42" t="s">
+      <c r="G61" s="44" t="s">
         <v>40</v>
-      </c>
-      <c r="E54" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="F54" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="G54" s="44" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="D54:G54"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <dataValidations xWindow="283" yWindow="632" count="5">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nesta coluna, insira o nome da pessoa designada a cada tarefa para o Dia 1." sqref="E4 E10 E17 E26 E33 E39" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nesta coluna, insira o nome da pessoa designada a cada tarefa para o Dia 2." sqref="G4 G10 G17 G26 G33 G39" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Clique duas vezes nas células sob esta coluna para marcar as tarefas como concluídas." sqref="F10 F4 F17 F26 F33 F39" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nesta coluna, insira o nome da pessoa designada a cada tarefa para o Dia 1." sqref="E4 E10 E17 E26 E33 E39 E47" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nesta coluna, insira o nome da pessoa designada a cada tarefa para o Dia 2." sqref="G4 G10 G17 G26 G33 G39 G47" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Clique duas vezes nas células sob esta coluna para marcar as tarefas como concluídas." sqref="F10 F4 F17 F26 F33 F39 F47" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira cada tarefa nesta coluna." sqref="D4 D10" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>$I$5:$I$7</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D45" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G49" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D52" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G56" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4323,7 +4547,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="47" id="{176E1538-9EFD-4E7F-8E7F-B77DEBB3E249}">
+          <x14:cfRule type="iconSet" priority="54" id="{176E1538-9EFD-4E7F-8E7F-B77DEBB3E249}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4342,7 +4566,7 @@
           <xm:sqref>F11:F12 H14:H17 J14:J17 L14:L17 N14:N17 P14:P17 R14:R17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="46" id="{5387C428-20DF-4FFE-AF1B-11F61B181753}">
+          <x14:cfRule type="iconSet" priority="53" id="{5387C428-20DF-4FFE-AF1B-11F61B181753}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4361,7 +4585,7 @@
           <xm:sqref>F18:F19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="49" id="{EE5E23B3-A11B-47B4-99A0-9EFEE1F5305B}">
+          <x14:cfRule type="iconSet" priority="56" id="{EE5E23B3-A11B-47B4-99A0-9EFEE1F5305B}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4380,7 +4604,7 @@
           <xm:sqref>F20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{25C42D9B-234A-4861-9413-3E46E9B672AD}">
+          <x14:cfRule type="iconSet" priority="10" id="{25C42D9B-234A-4861-9413-3E46E9B672AD}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4399,7 +4623,26 @@
           <xm:sqref>F21:F23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{F57CEF24-7066-4C2C-AFEE-CA63D1AE06C5}">
+          <x14:cfRule type="iconSet" priority="64" id="{6014A88C-DABB-4BC0-81D4-1C5CBAD85A84}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H5:H8 J5 L5 N5:N8 P5:P8 R5:R8 F5:F6</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="7" id="{63BE4E83-6FAD-4D9F-BF7A-ABC4D202AEB7}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4418,7 +4661,7 @@
           <xm:sqref>F27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{C9F2EBDE-B5B8-4675-A55A-821E6BB85053}">
+          <x14:cfRule type="iconSet" priority="6" id="{59849361-CC3E-4AAE-B850-C9DF9119EF09}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4434,10 +4677,29 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F28:F29</xm:sqref>
+          <xm:sqref>F28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="48" id="{C99C482E-AD63-4DC8-9816-C43254E14141}">
+          <x14:cfRule type="iconSet" priority="5" id="{C9E132D4-8BFA-48F4-9A94-BCE3578A8141}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>F29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{3AB04D59-B0FC-4518-9704-88CCDA457496}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4456,7 +4718,7 @@
           <xm:sqref>F34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="50" id="{F9FAE60C-EBC3-4D8D-B06F-97C2F9EF82E9}">
+          <x14:cfRule type="iconSet" priority="3" id="{CA139C56-C730-4E24-BED7-E52AC551B373}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4475,7 +4737,7 @@
           <xm:sqref>F35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{A4516B3C-180E-4E0C-9B74-FEBDA679F4DD}">
+          <x14:cfRule type="iconSet" priority="2" id="{CC4FEA51-2812-4C01-AAD2-45BCFD2F1973}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4491,10 +4753,10 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F40:F42</xm:sqref>
+          <xm:sqref>F48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="57" id="{6014A88C-DABB-4BC0-81D4-1C5CBAD85A84}">
+          <x14:cfRule type="iconSet" priority="1" id="{181E893A-A295-4905-B94F-268E89F4EDC8}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -4510,7 +4772,26 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>H5:H8 J5 L5 N5:N8 P5:P8 R5:R8 F5:F6</xm:sqref>
+          <xm:sqref>F49:F50</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="65" id="{A4516B3C-180E-4E0C-9B74-FEBDA679F4DD}">
+            <x14:iconSet iconSet="3Symbols2" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>F40:F46</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4519,6 +4800,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="9873e3eb-efbd-427c-b89e-18c992b24cb9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9240cd1e-e99b-4c38-a677-bfc3f12694be">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <ReferenceId xmlns="9240cd1e-e99b-4c38-a677-bfc3f12694be" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FD8FCE98A4A2A24ABDB27E7047C09FC5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="317e2298551f07e41f4e89cba2626dec">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9240cd1e-e99b-4c38-a677-bfc3f12694be" xmlns:ns3="9873e3eb-efbd-427c-b89e-18c992b24cb9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78ef13e1b7921191667c88cc6d3ea5c3" ns2:_="" ns3:_="">
     <xsd:import namespace="9240cd1e-e99b-4c38-a677-bfc3f12694be"/>
@@ -4719,18 +5012,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="9873e3eb-efbd-427c-b89e-18c992b24cb9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9240cd1e-e99b-4c38-a677-bfc3f12694be">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <ReferenceId xmlns="9240cd1e-e99b-4c38-a677-bfc3f12694be" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4741,25 +5022,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53ABF40-3749-4196-8749-49C14B284732}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9240cd1e-e99b-4c38-a677-bfc3f12694be"/>
-    <ds:schemaRef ds:uri="9873e3eb-efbd-427c-b89e-18c992b24cb9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61D8B24C-3B85-4379-80DC-A0BB54E539A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4779,6 +5041,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53ABF40-3749-4196-8749-49C14B284732}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9240cd1e-e99b-4c38-a677-bfc3f12694be"/>
+    <ds:schemaRef ds:uri="9873e3eb-efbd-427c-b89e-18c992b24cb9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E60A8B6F-A245-4A02-AD66-F6A27855DC90}">
   <ds:schemaRefs>

</xml_diff>